<commit_message>
updated the REST API and data model (User, Schedule, Appointment).
</commit_message>
<xml_diff>
--- a/doc/apiDBInfo.xlsx
+++ b/doc/apiDBInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laweng\Documents\vaccine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA44C3EC-1E80-4C60-9740-92BBAE554460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DEE2EF9-03BE-4CF0-AE3F-1751055191F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{81B81D6B-3760-4757-8F0E-9834F8F12BA3}"/>
+    <workbookView xWindow="4000" yWindow="870" windowWidth="14400" windowHeight="8530" xr2:uid="{81B81D6B-3760-4757-8F0E-9834F8F12BA3}"/>
   </bookViews>
   <sheets>
     <sheet name="API &amp; DB" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="91">
-  <si>
-    <t>REST API</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="100">
   <si>
     <t>URL</t>
   </si>
@@ -61,75 +58,24 @@
     <t>GET</t>
   </si>
   <si>
-    <t>/v1/vaccine/appointments/cancel?confirmationId:String</t>
-  </si>
-  <si>
     <t>UPDATE</t>
   </si>
   <si>
     <t>cancelStatus(confirmationId:String, cancelConfirmId:String)</t>
   </si>
   <si>
-    <t>/v1/vaccineCenter/getCenterInfo</t>
-  </si>
-  <si>
-    <t>/v1/vaccineCenter/getVaccineType</t>
-  </si>
-  <si>
-    <t>confirmationId:String,notifyType:String,notifyString:String</t>
-  </si>
-  <si>
     <t>notificationId:String</t>
   </si>
   <si>
     <t>User (name:String, address:String, officialId:String)</t>
   </si>
   <si>
-    <t>id:Long</t>
-  </si>
-  <si>
-    <t>/v1/vaccine/appointments/list?id:Long</t>
-  </si>
-  <si>
-    <t>List of(dateTime:DateTime,centerId:Integer,openSlot:int)</t>
-  </si>
-  <si>
     <t>confirmationStatus(booked:Boolean, centerId:Integer, confirmId:String)</t>
   </si>
   <si>
-    <t>List of (record:VaccineRecord(centerId:Integer, vaccineTypeId:Integer, date:Date, lot:String)</t>
-  </si>
-  <si>
-    <t>List of(dateTime:DateTime,centerId:Integer,vaccineTypeId:Integer)</t>
-  </si>
-  <si>
-    <t>List of(centerId:Integer, name:String, address:String)</t>
-  </si>
-  <si>
-    <t>List of(vaccineTypeId:Integer, name:String)</t>
-  </si>
-  <si>
-    <t>/v1/vaccine/appointment/setReminder</t>
-  </si>
-  <si>
-    <t>/v1/vaccineCenter/restock</t>
-  </si>
-  <si>
-    <t>/v1/vaccine/appointment/report?date:Date</t>
-  </si>
-  <si>
     <t>List of(center:Integer, vaccineTypeId:Integer, shotAdministered:int)</t>
   </si>
   <si>
-    <t>/v1/vaccine/appointment/completed</t>
-  </si>
-  <si>
-    <t>/v1/vaccine/appointments/book?date=&lt;date&gt;,time=&lt;time&gt;,centerId=&lt;centerId&gt;,vaccineTypeId=&lt;vaccineTypeId&gt;</t>
-  </si>
-  <si>
-    <t>/v1/vaccine/appointments/getFreeSlot?weekOf=&lt;monthDay&gt;,center=&lt;center&gt;,vaccineTypeId=&lt;vaccineTypeId&gt;</t>
-  </si>
-  <si>
     <t>DB Table</t>
   </si>
   <si>
@@ -205,12 +151,6 @@
     <t>Time</t>
   </si>
   <si>
-    <t>totalSlot</t>
-  </si>
-  <si>
-    <t>openSlot</t>
-  </si>
-  <si>
     <t>comfirmationId</t>
   </si>
   <si>
@@ -241,40 +181,16 @@
     <t>status</t>
   </si>
   <si>
-    <t>primary key, index(date)</t>
-  </si>
-  <si>
     <t>Inventory</t>
   </si>
   <si>
-    <t>count</t>
-  </si>
-  <si>
     <t>expiration</t>
   </si>
   <si>
-    <t>confirmationId:String,inventoryId:Integer</t>
-  </si>
-  <si>
     <t>OPEN/COMPLETED/CANCELLED</t>
   </si>
   <si>
     <t>cancelId</t>
-  </si>
-  <si>
-    <t>vaccineTypeId:Integer, Lot:String, expiration:Date, count:int,centerId:Integer</t>
-  </si>
-  <si>
-    <t>primary key (date, time, centerId, vaccineTypeId)</t>
-  </si>
-  <si>
-    <t>/v1/vaccine/user/register</t>
-  </si>
-  <si>
-    <t>/v1/vaccine/user/list</t>
-  </si>
-  <si>
-    <t>/v1/vaccine/user/list?id=Integer</t>
   </si>
   <si>
     <t>list of User (name:String, address:String, officialId:String)</t>
@@ -305,18 +221,137 @@
 If not, microservice needs to integrate with an external notification system.</t>
   </si>
   <si>
-    <t>/v1/vaccineCenter/appointment/publishReminder?date:Date</t>
-  </si>
-  <si>
-    <t>/v1/vaccine/appointments/certificate/get?userId:&lt;id&gt;</t>
+    <t>provider</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>vaccineId</t>
+  </si>
+  <si>
+    <t>lotSize</t>
+  </si>
+  <si>
+    <t>available</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
+    <t>List of Center(centerId:Integer, name:String, address:String,...)</t>
+  </si>
+  <si>
+    <t>Shipment(vaccineId:Integer, lot:String, lotSize:Integer, expiration:Date…)</t>
+  </si>
+  <si>
+    <t>/v1/vaccine/users/register</t>
+  </si>
+  <si>
+    <t>/v1/vaccine/users/list</t>
+  </si>
+  <si>
+    <t>/v1/vaccine/users/list?id=Integer</t>
+  </si>
+  <si>
+    <t>/v1/vaccineCenters/restock</t>
+  </si>
+  <si>
+    <t>/v1/vaccineCenters/listCenter</t>
+  </si>
+  <si>
+    <t>/v1/vaccineCenters/listVaccine</t>
+  </si>
+  <si>
+    <t>/v1/vaccineCenters/addCenter</t>
+  </si>
+  <si>
+    <t>/v1/vaccineCenters/addVaccineType</t>
+  </si>
+  <si>
+    <t>List of Vaccine(vaccineId:Integer, name:String, ...)</t>
+  </si>
+  <si>
+    <t>Center( name:String, address:String,…)</t>
+  </si>
+  <si>
+    <t>Vaccine(name:String, …)</t>
+  </si>
+  <si>
+    <t>Center with assigned id.</t>
+  </si>
+  <si>
+    <t>Vaccine with assigned id.</t>
+  </si>
+  <si>
+    <t>index(date, time, centerId, vaccineTypeId)</t>
+  </si>
+  <si>
+    <t>allocatedShot</t>
+  </si>
+  <si>
+    <t>availableShot</t>
+  </si>
+  <si>
+    <t>scheduleId</t>
+  </si>
+  <si>
+    <t>User with id populated</t>
+  </si>
+  <si>
+    <t>List of Appointment with Schedule(date:Date, time:Time,centerId:Integer,vaccineTypeId:Integer...))</t>
+  </si>
+  <si>
+    <t>List of (record:VaccineRecord(centerId:Integer, vaccineTypeId:Integer, date:Date, lot:String,certificate:String)</t>
+  </si>
+  <si>
+    <t>List of Schedule(id:Integer,date:Date,time:Time,centerId:Integer,availableShot:int...)</t>
+  </si>
+  <si>
+    <t>/v1/vaccine/appointments/completed?confirmationId=&lt;confirmationId:String&gt;,inventory=&lt;inventoryId:Integer&gt;</t>
+  </si>
+  <si>
+    <t>/v1/vaccine/appointments/report?date=&lt;date:Date&gt;</t>
+  </si>
+  <si>
+    <t>/v1/vaccine/appointments/certificate/get?userId=&lt;userId:Integer&gt;</t>
+  </si>
+  <si>
+    <t>/v1/vaccine/appointments/list?confirmationId=&lt;confirmationId:String&gt;</t>
+  </si>
+  <si>
+    <t>/v1/vaccine/appointments/cancel?confirmationId=&lt;confirmationId:String&gt;</t>
+  </si>
+  <si>
+    <t>/v1/vaccine/appointment/setReminder?confirmationId=&lt;confirmationId:String&gt;,notifyType=&lt;emailOrSMS:String&gt;,notifyString=&lt;emailAddrOrPhoneNumber:String&gt;</t>
+  </si>
+  <si>
+    <t>/v1/vaccine/appointments/book?scheduleId=&lt;scheduleId:Integer&gt;,userId=&lt;userId:Integer&gt;</t>
+  </si>
+  <si>
+    <t>/v1/vaccine/appointments/getFreeSlot?weekOf=&lt;monthDay:Date&gt;,center=&lt;centerId:Integer&gt;,vaccineId=&lt;vaccineId:Integer&gt;</t>
+  </si>
+  <si>
+    <t>/v1/vaccineCenters/publishReminder?date=&lt;date:Date&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -344,11 +379,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,640 +699,700 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5CDD7C2-B249-4E36-9563-13CFE4F4DA6E}">
-  <dimension ref="A2:D68"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:XFD46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="74.453125" customWidth="1"/>
+    <col min="1" max="1" width="59.26953125" customWidth="1"/>
     <col min="2" max="2" width="50.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>80</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>94</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
-      <c r="D13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>84</v>
-      </c>
-      <c r="B17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" t="s">
-        <v>81</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>77</v>
+      </c>
+      <c r="B20" t="s">
+        <v>80</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="C23" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="D29" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="D31" t="s">
-        <v>41</v>
-      </c>
-    </row>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="C34" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="D34" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="D35" t="s">
-        <v>41</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>45</v>
-      </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="C37" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D37" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B38" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" t="s">
-        <v>40</v>
-      </c>
-      <c r="D38" t="s">
-        <v>41</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>47</v>
-      </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="C40" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="D40" t="s">
-        <v>76</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D41" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D42" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B43" t="s">
-        <v>54</v>
-      </c>
-      <c r="C43" t="s">
-        <v>55</v>
-      </c>
-      <c r="D43" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>29</v>
+      </c>
       <c r="B44" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>36</v>
+        <v>18</v>
+      </c>
+      <c r="D44" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C45" t="s">
+        <v>31</v>
+      </c>
+      <c r="D45" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
         <v>36</v>
       </c>
+      <c r="C46" t="s">
+        <v>37</v>
+      </c>
+      <c r="D46" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>46</v>
-      </c>
       <c r="B47" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="C47" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="D47" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="C48" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="D48" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C49" t="s">
-        <v>49</v>
-      </c>
-      <c r="D49" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="C50" t="s">
-        <v>55</v>
-      </c>
-      <c r="D50" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B51" t="s">
-        <v>50</v>
-      </c>
-      <c r="C51" t="s">
-        <v>36</v>
-      </c>
-      <c r="D51" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>28</v>
+      </c>
       <c r="B52" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="C52" t="s">
-        <v>40</v>
+        <v>22</v>
+      </c>
+      <c r="D52" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="C53" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="C54" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="D54" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="C55" t="s">
-        <v>40</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B56" t="s">
+        <v>42</v>
+      </c>
+      <c r="C56" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>63</v>
-      </c>
       <c r="B57" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C57" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D57" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C58" t="s">
-        <v>40</v>
-      </c>
-      <c r="D58" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B59" t="s">
-        <v>51</v>
-      </c>
-      <c r="C59" t="s">
-        <v>36</v>
-      </c>
-      <c r="D59" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>43</v>
+      </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="C60" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="D60" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C61" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="D61" t="s">
-        <v>41</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B62" t="s">
+        <v>33</v>
+      </c>
+      <c r="C62" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>69</v>
-      </c>
       <c r="B63" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="C63" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D63" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C64" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D64" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B65" t="s">
-        <v>66</v>
-      </c>
-      <c r="C65" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>48</v>
+      </c>
       <c r="B66" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="C66" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="D66" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C67" t="s">
+        <v>18</v>
+      </c>
+      <c r="D67" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B68" t="s">
+        <v>46</v>
+      </c>
+      <c r="C68" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B69" t="s">
+        <v>64</v>
+      </c>
+      <c r="C69" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B70" t="s">
+        <v>65</v>
+      </c>
+      <c r="C70" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B71" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B68" t="s">
-        <v>50</v>
-      </c>
-      <c r="C68" t="s">
-        <v>36</v>
-      </c>
-      <c r="D68" t="s">
-        <v>52</v>
+      <c r="C71" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B72" t="s">
+        <v>32</v>
+      </c>
+      <c r="C72" t="s">
+        <v>18</v>
+      </c>
+      <c r="D72" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1315,7 +1411,7 @@
   <sheetData>
     <row r="2" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated Appointment and Schedule attribute as well as moved Certitificate to User service.
</commit_message>
<xml_diff>
--- a/doc/apiDBInfo.xlsx
+++ b/doc/apiDBInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laweng\Documents\vaccine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DEE2EF9-03BE-4CF0-AE3F-1751055191F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D6F692-F2E3-496E-8543-1623B2AED08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="870" windowWidth="14400" windowHeight="8530" xr2:uid="{81B81D6B-3760-4757-8F0E-9834F8F12BA3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{81B81D6B-3760-4757-8F0E-9834F8F12BA3}"/>
   </bookViews>
   <sheets>
     <sheet name="API &amp; DB" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="101">
   <si>
     <t>URL</t>
   </si>
@@ -136,9 +136,6 @@
     <t>centerId</t>
   </si>
   <si>
-    <t>vaccineTypeId</t>
-  </si>
-  <si>
     <t>Center.id</t>
   </si>
   <si>
@@ -169,12 +166,6 @@
     <t>Certificate</t>
   </si>
   <si>
-    <t>User.id(primary key)</t>
-  </si>
-  <si>
-    <t>certificateId</t>
-  </si>
-  <si>
     <t>lot</t>
   </si>
   <si>
@@ -209,9 +200,6 @@
   </si>
   <si>
     <t>vaccineInventory (trigger to update available schedule due to new inventory)</t>
-  </si>
-  <si>
-    <t>inventoryId:Integer</t>
   </si>
   <si>
     <t>shotAdministrated (reduce the count in inventory)</t>
@@ -254,9 +242,6 @@
     <t>/v1/vaccine/users/list</t>
   </si>
   <si>
-    <t>/v1/vaccine/users/list?id=Integer</t>
-  </si>
-  <si>
     <t>/v1/vaccineCenters/restock</t>
   </si>
   <si>
@@ -287,9 +272,6 @@
     <t>Vaccine with assigned id.</t>
   </si>
   <si>
-    <t>index(date, time, centerId, vaccineTypeId)</t>
-  </si>
-  <si>
     <t>allocatedShot</t>
   </si>
   <si>
@@ -305,21 +287,12 @@
     <t>List of Appointment with Schedule(date:Date, time:Time,centerId:Integer,vaccineTypeId:Integer...))</t>
   </si>
   <si>
-    <t>List of (record:VaccineRecord(centerId:Integer, vaccineTypeId:Integer, date:Date, lot:String,certificate:String)</t>
-  </si>
-  <si>
     <t>List of Schedule(id:Integer,date:Date,time:Time,centerId:Integer,availableShot:int...)</t>
   </si>
   <si>
-    <t>/v1/vaccine/appointments/completed?confirmationId=&lt;confirmationId:String&gt;,inventory=&lt;inventoryId:Integer&gt;</t>
-  </si>
-  <si>
     <t>/v1/vaccine/appointments/report?date=&lt;date:Date&gt;</t>
   </si>
   <si>
-    <t>/v1/vaccine/appointments/certificate/get?userId=&lt;userId:Integer&gt;</t>
-  </si>
-  <si>
     <t>/v1/vaccine/appointments/list?confirmationId=&lt;confirmationId:String&gt;</t>
   </si>
   <si>
@@ -336,6 +309,36 @@
   </si>
   <si>
     <t>/v1/vaccineCenters/publishReminder?date=&lt;date:Date&gt;</t>
+  </si>
+  <si>
+    <t>/v1/vaccine/users/list?id:Integer</t>
+  </si>
+  <si>
+    <t>index:userId</t>
+  </si>
+  <si>
+    <t>non-null, Vaccine.id</t>
+  </si>
+  <si>
+    <t>index(date, time, centerId, vaccineId)</t>
+  </si>
+  <si>
+    <t>non-null, Center.id</t>
+  </si>
+  <si>
+    <t>/v1/vaccine/users/retrieveCertificate?userId=&lt;userId:Integer&gt;</t>
+  </si>
+  <si>
+    <t>List of Certificate</t>
+  </si>
+  <si>
+    <t>/v1/vaccine/appointments/completed?confirmationId=&lt;confirmationId:String&gt;,vaccineId:Integer,lot:String,inventory=&lt;inventoryId:Integer&gt;</t>
+  </si>
+  <si>
+    <t>inventoryId:Integer,vaccineId:Integer, lot:String,userId:Integer</t>
+  </si>
+  <si>
+    <t>inventoryId:Integer,vaccineId:Integer, lot:String, userId:Integer</t>
   </si>
 </sst>
 </file>
@@ -699,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5CDD7C2-B249-4E36-9563-13CFE4F4DA6E}">
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:XFD46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -729,7 +732,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -738,23 +741,23 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -763,274 +766,259 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
-        <v>90</v>
+      <c r="D5" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>99</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>88</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>89</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" t="s">
-        <v>54</v>
+        <v>98</v>
       </c>
       <c r="C15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" t="s">
-        <v>53</v>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
+      <c r="D22" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>13</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>14</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B30" t="s">
         <v>15</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C30" t="s">
         <v>16</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D30" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>17</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B31" t="s">
         <v>5</v>
       </c>
-      <c r="C28" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B29" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
         <v>21</v>
       </c>
-      <c r="C29" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B30" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
         <v>24</v>
       </c>
-      <c r="C30" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B31" t="s">
+      <c r="C33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
         <v>25</v>
-      </c>
-      <c r="C31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B34" t="s">
-        <v>21</v>
       </c>
       <c r="C34" t="s">
         <v>22</v>
@@ -1039,31 +1027,24 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B35" t="s">
-        <v>24</v>
-      </c>
-      <c r="C35" t="s">
-        <v>22</v>
-      </c>
-      <c r="D35" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>26</v>
+      </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D36" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="C37" t="s">
         <v>22</v>
@@ -1072,23 +1053,31 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>27</v>
-      </c>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="C39" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D39" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="C40" t="s">
         <v>22</v>
@@ -1097,297 +1086,328 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B41" t="s">
-        <v>61</v>
-      </c>
-      <c r="C41" t="s">
-        <v>22</v>
-      </c>
-      <c r="D41" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B42" t="s">
-        <v>62</v>
-      </c>
-      <c r="C42" t="s">
-        <v>22</v>
-      </c>
-      <c r="D42" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>58</v>
+      </c>
+      <c r="C45" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>29</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B47" t="s">
         <v>5</v>
       </c>
-      <c r="C44" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="C47" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B45" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
         <v>30</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C48" t="s">
         <v>31</v>
       </c>
-      <c r="D45" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B46" t="s">
+      <c r="D48" t="s">
+        <v>23</v>
+      </c>
+      <c r="E48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>35</v>
+      </c>
+      <c r="C49" t="s">
         <v>36</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D49" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D50" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B51" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B53" t="s">
+        <v>79</v>
+      </c>
+      <c r="C53" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>28</v>
+      </c>
+      <c r="B55" t="s">
         <v>37</v>
       </c>
-      <c r="D46" t="s">
+      <c r="C55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B56" t="s">
+        <v>38</v>
+      </c>
+      <c r="C56" t="s">
+        <v>18</v>
+      </c>
+      <c r="D56" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B57" t="s">
+        <v>80</v>
+      </c>
+      <c r="C57" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B47" t="s">
-        <v>32</v>
-      </c>
-      <c r="C47" t="s">
-        <v>18</v>
-      </c>
-      <c r="D47" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B48" t="s">
-        <v>33</v>
-      </c>
-      <c r="C48" t="s">
-        <v>18</v>
-      </c>
-      <c r="D48" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B49" t="s">
-        <v>84</v>
-      </c>
-      <c r="C49" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B50" t="s">
-        <v>85</v>
-      </c>
-      <c r="C50" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>28</v>
-      </c>
-      <c r="B52" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B58" t="s">
+        <v>40</v>
+      </c>
+      <c r="C58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B59" t="s">
+        <v>41</v>
+      </c>
+      <c r="C59" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B60" t="s">
+        <v>44</v>
+      </c>
+      <c r="C60" t="s">
+        <v>22</v>
+      </c>
+      <c r="D60" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B61" t="s">
+        <v>48</v>
+      </c>
+      <c r="C61" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>42</v>
+      </c>
+      <c r="B63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" t="s">
+        <v>22</v>
+      </c>
+      <c r="D63" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B64" t="s">
         <v>38</v>
       </c>
-      <c r="C52" t="s">
-        <v>22</v>
-      </c>
-      <c r="D52" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B53" t="s">
-        <v>39</v>
-      </c>
-      <c r="C53" t="s">
-        <v>18</v>
-      </c>
-      <c r="D53" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B54" t="s">
-        <v>86</v>
-      </c>
-      <c r="C54" t="s">
-        <v>18</v>
-      </c>
-      <c r="D54" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B55" t="s">
-        <v>41</v>
-      </c>
-      <c r="C55" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B56" t="s">
-        <v>42</v>
-      </c>
-      <c r="C56" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B57" t="s">
-        <v>47</v>
-      </c>
-      <c r="C57" t="s">
-        <v>22</v>
-      </c>
-      <c r="D57" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B58" t="s">
-        <v>51</v>
-      </c>
-      <c r="C58" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>43</v>
-      </c>
-      <c r="B60" t="s">
-        <v>39</v>
-      </c>
-      <c r="C60" t="s">
-        <v>18</v>
-      </c>
-      <c r="D60" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B61" t="s">
-        <v>45</v>
-      </c>
-      <c r="C61" t="s">
-        <v>22</v>
-      </c>
-      <c r="D61" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B62" t="s">
-        <v>33</v>
-      </c>
-      <c r="C62" t="s">
-        <v>18</v>
-      </c>
-      <c r="D62" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B63" t="s">
-        <v>46</v>
-      </c>
-      <c r="C63" t="s">
-        <v>22</v>
-      </c>
-      <c r="D63" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B64" t="s">
-        <v>30</v>
-      </c>
       <c r="C64" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="D64" t="s">
         <v>23</v>
       </c>
+      <c r="E64" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B65" t="s">
+        <v>59</v>
+      </c>
+      <c r="C65" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>48</v>
-      </c>
       <c r="B66" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="C66" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D66" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="C67" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D67" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B68" t="s">
-        <v>46</v>
-      </c>
-      <c r="C68" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>45</v>
+      </c>
       <c r="B69" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
       <c r="C69" t="s">
         <v>18</v>
+      </c>
+      <c r="D69" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C70" t="s">
         <v>18</v>
+      </c>
+      <c r="D70" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C71" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B72" t="s">
+        <v>60</v>
+      </c>
+      <c r="C72" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B73" t="s">
+        <v>61</v>
+      </c>
+      <c r="C73" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B74" t="s">
+        <v>46</v>
+      </c>
+      <c r="C74" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B75" t="s">
         <v>32</v>
       </c>
-      <c r="C72" t="s">
-        <v>18</v>
-      </c>
-      <c r="D72" t="s">
-        <v>34</v>
+      <c r="C75" t="s">
+        <v>18</v>
+      </c>
+      <c r="D75" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1411,7 +1431,7 @@
   <sheetData>
     <row r="2" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>